<commit_message>
Login concept is added
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -2,21 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="669" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="669" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LocatorStrategy" sheetId="31" r:id="rId1"/>
-    <sheet name="HomePage" sheetId="30" r:id="rId2"/>
-    <sheet name="UsersPage" sheetId="32" r:id="rId3"/>
+    <sheet name="LoginPage" sheetId="34" r:id="rId2"/>
+    <sheet name="HomePage" sheetId="30" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Element Name</t>
   </si>
@@ -51,68 +56,47 @@
     <t>Locator Strategy</t>
   </si>
   <si>
-    <t>//input[@name='q']</t>
-  </si>
-  <si>
-    <t>search_bar</t>
-  </si>
-  <si>
-    <t>//a[@href='/questions/ask']</t>
-  </si>
-  <si>
-    <t>//button[@type='submit']//*[@class='svg-icon iconSearch']</t>
-  </si>
-  <si>
-    <t>btn_search</t>
-  </si>
-  <si>
-    <t>btn_ask_question</t>
-  </si>
-  <si>
-    <t>nav-users</t>
-  </si>
-  <si>
-    <t>nav_bar_users_menu</t>
-  </si>
-  <si>
-    <t>userfilter</t>
-  </si>
-  <si>
-    <t>txt_box_user_search</t>
-  </si>
-  <si>
-    <t>//a[text()='Osanda Deshan']</t>
-  </si>
-  <si>
-    <t>lbl_seach_result</t>
-  </si>
-  <si>
-    <t>//a[@title='How to automate Android 6.0 Date picker to set any date?']</t>
-  </si>
-  <si>
-    <t>test_search_result</t>
-  </si>
-  <si>
-    <t>//a[@title='searchText']</t>
-  </si>
-  <si>
-    <t>//span[@class='-link--channel-name']</t>
-  </si>
-  <si>
-    <t>nav_bar_stackoverflow_menu</t>
-  </si>
-  <si>
-    <t>//a[@class='pl8 js-gps-track nav-links--link']</t>
-  </si>
-  <si>
-    <t>nav_bar_home_menu</t>
+    <t>txt_email</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>passwd</t>
+  </si>
+  <si>
+    <t>txt_password</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Sign in')]</t>
+  </si>
+  <si>
+    <t>SubmitLogin</t>
+  </si>
+  <si>
+    <t>btn_submit</t>
+  </si>
+  <si>
+    <t>lbl_profile_name</t>
+  </si>
+  <si>
+    <t>//span[text()='profileName']</t>
+  </si>
+  <si>
+    <t>nav_bar_signout_link</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Sign out')]</t>
+  </si>
+  <si>
+    <t>nav_bar_signin_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -129,6 +113,18 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -181,8 +177,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -209,7 +221,23 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -236,7 +264,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1">
+  <tableStyles count="1" defaultPivotStyle="PivotStyleMedium4">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
@@ -1485,26 +1513,190 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IR20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.85546875" style="8" customWidth="1"/>
+    <col min="4" max="252" width="8.85546875" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>LocatorStrategy!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IS21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="253" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1521,13 +1713,13 @@
     </row>
     <row r="2" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -1782,80 +1974,50 @@
     </row>
     <row r="3" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
+      <c r="A4" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1919,7 +2081,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1934,160 +2096,8 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IR20"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.85546875" style="8" customWidth="1"/>
-    <col min="4" max="252" width="8.85546875" style="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>LocatorStrategy!$A$2:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B20</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
Tabs and window operations added
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="669" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="669" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LocatorStrategy" sheetId="31" r:id="rId1"/>
     <sheet name="LoginPage" sheetId="34" r:id="rId2"/>
     <sheet name="HomePage" sheetId="30" r:id="rId3"/>
+    <sheet name="UploadPage" sheetId="36" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Element Name</t>
   </si>
@@ -114,6 +116,42 @@
   </si>
   <si>
     <t>lbl_search_result_locator</t>
+  </si>
+  <si>
+    <t>inputfile</t>
+  </si>
+  <si>
+    <t>//button[contains(text(),'Upload')]</t>
+  </si>
+  <si>
+    <t>uploadfile_0</t>
+  </si>
+  <si>
+    <t>terms</t>
+  </si>
+  <si>
+    <t>send</t>
+  </si>
+  <si>
+    <t>//*[contains(text(), '1 file')]</t>
+  </si>
+  <si>
+    <t>lbl_upload_success</t>
+  </si>
+  <si>
+    <t>btn_upload_file</t>
+  </si>
+  <si>
+    <t>btn_terms</t>
+  </si>
+  <si>
+    <t>btn_test_upload</t>
+  </si>
+  <si>
+    <t>btn_upload</t>
+  </si>
+  <si>
+    <t>btn_choose_file</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IS21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -2149,4 +2187,176 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IS21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="253" width="8.85546875" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>